<commit_message>
working acdc combined 3 node system
</commit_message>
<xml_diff>
--- a/data/case24_ieee_rts_DC.xlsx
+++ b/data/case24_ieee_rts_DC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samho\Desktop\PhD\DC OPF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6563634B-AC16-461F-A767-DB7D133D9D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F642732A-474F-4729-A838-AEBDE67927C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ac_links" sheetId="13" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -110,9 +110,6 @@
     <t>20</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>busname</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
   </si>
   <si>
     <t>180</t>
-  </si>
-  <si>
-    <t>37</t>
   </si>
   <si>
     <t>175</t>
@@ -1021,7 +1015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F45778F-8D79-4B69-AE3A-F144DB1573E9}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1032,48 +1026,48 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" t="s">
-        <v>43</v>
-      </c>
       <c r="L1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M1" t="s">
         <v>2</v>
       </c>
       <c r="N1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1109,7 +1103,7 @@
         <v>1E-4</v>
       </c>
       <c r="M2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1117,7 +1111,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1153,7 +1147,7 @@
         <v>1E-4</v>
       </c>
       <c r="M3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N3">
         <v>20</v>
@@ -1177,7 +1171,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -1206,7 +1200,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B1" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -1227,16 +1221,16 @@
     </row>
     <row r="2" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1258,13 +1252,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R3" s="6"/>
     </row>
@@ -1273,13 +1267,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R4" s="6"/>
     </row>
@@ -1288,13 +1282,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R5" s="6"/>
     </row>
@@ -1303,13 +1297,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R6" s="6"/>
     </row>
@@ -1318,13 +1312,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R7" s="6"/>
     </row>
@@ -1333,13 +1327,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R8" s="6"/>
     </row>
@@ -1348,13 +1342,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R9" s="6"/>
     </row>
@@ -1363,13 +1357,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R10" s="6"/>
     </row>
@@ -1378,13 +1372,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R11" s="6"/>
     </row>
@@ -1393,13 +1387,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1447,7 +1441,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1486,36 +1480,36 @@
         <v>3</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="J1" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>115</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" s="20">
         <v>3</v>
@@ -1807,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1821,33 +1815,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>20</v>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>10</v>
@@ -1858,16 +1852,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -1878,16 +1872,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1980,45 +1974,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
@@ -2030,25 +2024,25 @@
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="L2" s="3">
         <v>0</v>
@@ -2059,7 +2053,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -2071,25 +2065,25 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
         <v>53</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>54</v>
       </c>
-      <c r="G3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" t="s">
-        <v>56</v>
-      </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -2100,7 +2094,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -2112,25 +2106,25 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
         <v>58</v>
       </c>
-      <c r="F4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -2294,60 +2288,60 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -2362,34 +2356,34 @@
         <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P2" s="3">
         <v>1.1000000000000001</v>
@@ -2454,43 +2448,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" t="s">
         <v>79</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="M1" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2514,19 +2508,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2534,7 +2528,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -2567,19 +2561,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2593,7 +2587,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2603,79 +2597,79 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y1" t="s">
         <v>79</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="X1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
@@ -2683,7 +2677,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -2711,7 +2705,7 @@
         <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L2">
         <v>100</v>
@@ -2726,7 +2720,7 @@
         <v>2</v>
       </c>
       <c r="P2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q2" t="s">
         <v>12</v>
@@ -2744,10 +2738,10 @@
         <v>12</v>
       </c>
       <c r="V2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="W2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="X2">
         <v>40</v>

</xml_diff>